<commit_message>
Experiment 01 - LLMs in TCM to MBT initial commit
</commit_message>
<xml_diff>
--- a/output/xlsx/RF001 - Autenticar Usuário--GT-.xlsx
+++ b/output/xlsx/RF001 - Autenticar Usuário--GT-.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">System: </t>
   </si>
   <si>
-    <t>RGP-Competências</t>
+    <t>GTI-Competências</t>
   </si>
   <si>
     <t/>
@@ -826,7 +826,7 @@
         <v>2.0</v>
       </c>
       <c r="B31" t="s" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s" s="6">
         <v>2</v>

</xml_diff>